<commit_message>
anillo 2 y 3
Aportes de elian. anillos en cuatitlan y tultitlan con enlaces para conectarse a satelite
</commit_message>
<xml_diff>
--- a/anillos.xlsx
+++ b/anillos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\Documents\GitHub\red_ibero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39DCB20-3B69-4379-AAB0-9190313DC19F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79974A0-0E1A-4A6C-B653-FBFD5828478E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4065" yWindow="4035" windowWidth="14955" windowHeight="11565" xr2:uid="{73DE5C8D-3A31-544E-881E-C7850F3F99F6}"/>
+    <workbookView xWindow="9405" yWindow="4035" windowWidth="14955" windowHeight="11565" xr2:uid="{73DE5C8D-3A31-544E-881E-C7850F3F99F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Site 1</t>
   </si>
@@ -113,7 +113,22 @@
     <t>hipodromo de las americas</t>
   </si>
   <si>
-    <t>lo llame anillo x</t>
+    <t>tec edomex</t>
+  </si>
+  <si>
+    <t>ford cuatitlan</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>kio tultitlan</t>
   </si>
 </sst>
 </file>
@@ -474,7 +489,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -510,17 +525,32 @@
         <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>